<commit_message>
Excel session 3 updated and zip ws
</commit_message>
<xml_diff>
--- a/Practica3 2024.eng/times.xlsx
+++ b/Practica3 2024.eng/times.xlsx
@@ -19,20 +19,49 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="9">
   <si>
     <t>n</t>
   </si>
   <si>
     <t>time(ms)</t>
+  </si>
+  <si>
+    <t>Oot</t>
+  </si>
+  <si>
+    <t>Substraction4</t>
+  </si>
+  <si>
+    <t>Substraction5</t>
+  </si>
+  <si>
+    <t>division4</t>
+  </si>
+  <si>
+    <t>Division5</t>
+  </si>
+  <si>
+    <t>size = 5</t>
+  </si>
+  <si>
+    <t>size = 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -60,8 +89,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -342,10 +373,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -357,6 +388,12 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="F1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
@@ -364,6 +401,12 @@
       </c>
       <c r="B2">
         <v>50</v>
+      </c>
+      <c r="F2" s="1">
+        <v>30</v>
+      </c>
+      <c r="G2" s="2">
+        <v>582</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -374,6 +417,13 @@
       <c r="B3">
         <v>377</v>
       </c>
+      <c r="F3" s="2">
+        <f>F2*$J$3</f>
+        <v>60</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1729</v>
+      </c>
       <c r="J3">
         <v>2</v>
       </c>
@@ -386,6 +436,13 @@
       <c r="B4">
         <v>2940</v>
       </c>
+      <c r="F4" s="2">
+        <f t="shared" ref="F4:F9" si="1">F3*$J$3</f>
+        <v>120</v>
+      </c>
+      <c r="G4" s="2">
+        <v>5305</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -395,29 +452,223 @@
       <c r="B5">
         <v>23661</v>
       </c>
+      <c r="F5" s="2">
+        <f t="shared" si="1"/>
+        <v>240</v>
+      </c>
+      <c r="G5" s="2">
+        <v>16138</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>1600</v>
       </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="2">
+        <f t="shared" si="1"/>
+        <v>480</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>3200</v>
       </c>
+      <c r="F7" s="2">
+        <f t="shared" si="1"/>
+        <v>960</v>
+      </c>
+      <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>6400</v>
       </c>
+      <c r="F8" s="2">
+        <f t="shared" si="1"/>
+        <v>1920</v>
+      </c>
+      <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>12800</v>
+      </c>
+      <c r="F9" s="2">
+        <f t="shared" si="1"/>
+        <v>3840</v>
+      </c>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" t="s">
+        <v>0</v>
+      </c>
+      <c r="G14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1000</v>
+      </c>
+      <c r="B15">
+        <v>65</v>
+      </c>
+      <c r="F15">
+        <v>1000</v>
+      </c>
+      <c r="G15">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f>A15*$J$3</f>
+        <v>2000</v>
+      </c>
+      <c r="B16">
+        <v>187</v>
+      </c>
+      <c r="F16">
+        <f>F15*$J$3</f>
+        <v>2000</v>
+      </c>
+      <c r="G16">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" ref="A17:A22" si="2">A16*$J$3</f>
+        <v>4000</v>
+      </c>
+      <c r="B17">
+        <v>739</v>
+      </c>
+      <c r="F17">
+        <f t="shared" ref="F17:F22" si="3">F16*$J$3</f>
+        <v>4000</v>
+      </c>
+      <c r="G17">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="2"/>
+        <v>8000</v>
+      </c>
+      <c r="B18">
+        <v>2954</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="3"/>
+        <v>8000</v>
+      </c>
+      <c r="G18">
+        <v>2994</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="shared" si="2"/>
+        <v>16000</v>
+      </c>
+      <c r="B19">
+        <v>11953</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="3"/>
+        <v>16000</v>
+      </c>
+      <c r="G19">
+        <v>2096</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="shared" si="2"/>
+        <v>32000</v>
+      </c>
+      <c r="B20">
+        <v>47034</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="3"/>
+        <v>32000</v>
+      </c>
+      <c r="G20">
+        <v>9108</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f t="shared" si="2"/>
+        <v>64000</v>
+      </c>
+      <c r="B21" t="s">
+        <v>2</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="3"/>
+        <v>64000</v>
+      </c>
+      <c r="G21">
+        <v>9108</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f t="shared" si="2"/>
+        <v>128000</v>
+      </c>
+      <c r="B22" t="s">
+        <v>2</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="3"/>
+        <v>128000</v>
+      </c>
+      <c r="G22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23" t="s">
+        <v>6</v>
+      </c>
+      <c r="G23" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>